<commit_message>
Khao sat SP lien quan
</commit_message>
<xml_diff>
--- a/Documents/Bảng-kế-hoạch-TLCN.xlsx
+++ b/Documents/Bảng-kế-hoạch-TLCN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nam4\TLCN-Xay-dung-website-ban-my-pham-pham\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Tran\Documents\TLCN\TLCN-Xay-dung-website-ban-my-pham\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22ED88-7A14-453C-B010-D657F7BDF37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B661ABF-7B50-414F-A62E-A728B39EABA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A498582B-0E29-459F-B17C-ACAF163EE552}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A498582B-0E29-459F-B17C-ACAF163EE552}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -775,24 +775,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7C54CA-71C9-4527-A841-C8DE308978A6}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
@@ -806,7 +806,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -820,10 +820,10 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -869,7 +869,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -895,11 +895,11 @@
         <v>44074</v>
       </c>
       <c r="I7" s="9">
-        <v>44093</v>
+        <v>44095</v>
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -927,7 +927,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
@@ -949,7 +949,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -975,7 +975,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1001,7 +1001,7 @@
       <c r="I11" s="9"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="s">
@@ -1045,7 +1045,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>6</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
@@ -1089,7 +1089,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="s">
@@ -1109,7 +1109,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
@@ -1129,7 +1129,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="8" t="s">
@@ -1149,7 +1149,7 @@
       <c r="I18" s="9"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
@@ -1169,7 +1169,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
@@ -1189,7 +1189,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
@@ -1209,7 +1209,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
@@ -1229,7 +1229,7 @@
       <c r="I22" s="9"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6" t="s">
@@ -1249,7 +1249,7 @@
       <c r="I23" s="9"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6" t="s">
@@ -1269,7 +1269,7 @@
       <c r="I24" s="9"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6" t="s">
@@ -1291,7 +1291,7 @@
       <c r="I25" s="9"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6" t="s">
@@ -1313,7 +1313,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>7</v>
       </c>
@@ -1337,7 +1337,7 @@
       <c r="I27" s="9"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>8</v>
       </c>
@@ -1363,7 +1363,7 @@
       <c r="I28" s="9"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
update ngày hoàn thành usecase
</commit_message>
<xml_diff>
--- a/Documents/Bảng-kế-hoạch-TLCN.xlsx
+++ b/Documents/Bảng-kế-hoạch-TLCN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nam4\TLCN-Xay-dung-website-ban-my-pham-pham\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Tran\Documents\TLCN\TLCN-Xay-dung-website-ban-my-pham\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA5222D-C5D7-468A-9484-C6499BDAFAB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C1DB4A-E419-460E-9BDA-3C0F11464D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A498582B-0E29-459F-B17C-ACAF163EE552}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A498582B-0E29-459F-B17C-ACAF163EE552}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -778,24 +778,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7C54CA-71C9-4527-A841-C8DE308978A6}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.88671875" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
@@ -809,7 +809,7 @@
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -823,10 +823,10 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
@@ -840,7 +840,7 @@
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -872,7 +872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -902,7 +902,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -932,7 +932,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
@@ -950,11 +950,13 @@
       <c r="G9" s="9">
         <v>44096</v>
       </c>
-      <c r="H9" s="9"/>
+      <c r="H9" s="9">
+        <v>44095</v>
+      </c>
       <c r="I9" s="9"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -976,11 +978,13 @@
       <c r="G10" s="9">
         <v>44099</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="9">
+        <v>44097</v>
+      </c>
       <c r="I10" s="9"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1002,11 +1006,13 @@
       <c r="G11" s="9">
         <v>44101</v>
       </c>
-      <c r="H11" s="9"/>
+      <c r="H11" s="9">
+        <v>44095</v>
+      </c>
       <c r="I11" s="9"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1030,7 +1036,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6" t="s">
@@ -1050,7 +1056,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>6</v>
       </c>
@@ -1074,7 +1080,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6" t="s">
@@ -1094,7 +1100,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6" t="s">
@@ -1114,7 +1120,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
@@ -1134,7 +1140,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="8" t="s">
@@ -1154,7 +1160,7 @@
       <c r="I18" s="9"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6" t="s">
@@ -1174,7 +1180,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="6" t="s">
@@ -1194,7 +1200,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6" t="s">
@@ -1214,7 +1220,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
@@ -1234,7 +1240,7 @@
       <c r="I22" s="9"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6" t="s">
@@ -1254,7 +1260,7 @@
       <c r="I23" s="9"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6" t="s">
@@ -1274,7 +1280,7 @@
       <c r="I24" s="9"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6" t="s">
@@ -1296,7 +1302,7 @@
       <c r="I25" s="9"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6" t="s">
@@ -1318,7 +1324,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>7</v>
       </c>
@@ -1342,7 +1348,7 @@
       <c r="I27" s="9"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>8</v>
       </c>
@@ -1368,7 +1374,7 @@
       <c r="I28" s="9"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Form Add New Product
</commit_message>
<xml_diff>
--- a/Documents/Bảng-kế-hoạch-TLCN.xlsx
+++ b/Documents/Bảng-kế-hoạch-TLCN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nam4\TLCN-Xay-dung-website-ban-my-pham-pham\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han Tran\Documents\TLCN\TLCN-Xay-dung-website-ban-my-pham\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74480DEC-A99C-44E3-BC9E-1644571D8325}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88ED1E2E-EC19-492A-B013-287E79CAF2DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A498582B-0E29-459F-B17C-ACAF163EE552}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A498582B-0E29-459F-B17C-ACAF163EE552}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
   <si>
     <t>STT</t>
   </si>
@@ -165,6 +165,33 @@
   </si>
   <si>
     <t>21/09</t>
+  </si>
+  <si>
+    <t>Xây dựng phương thức phân trang</t>
+  </si>
+  <si>
+    <t>Xây dựng phương thức cập nhật sản phẩm</t>
+  </si>
+  <si>
+    <t>Xây dựng phương thức quản lý ảnh</t>
+  </si>
+  <si>
+    <t>Tạo Web API project</t>
+  </si>
+  <si>
+    <t>Tạo RESTful API</t>
+  </si>
+  <si>
+    <t>Tạo API Quản lý ảnh</t>
+  </si>
+  <si>
+    <t>Tạo API Đăng nhập và Đăng ký</t>
+  </si>
+  <si>
+    <t>Bổ sung</t>
+  </si>
+  <si>
+    <t>Danh sách Người dùng</t>
   </si>
 </sst>
 </file>
@@ -461,8 +488,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{291BAA9C-8D41-439A-829B-432D695C79A1}" name="Table3" displayName="Table3" ref="A6:J29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
-  <autoFilter ref="A6:J29" xr:uid="{26FC5017-267D-4082-A3A9-95ECD173F855}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{291BAA9C-8D41-439A-829B-432D695C79A1}" name="Table3" displayName="Table3" ref="A6:J38" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A6:J38" xr:uid="{26FC5017-267D-4082-A3A9-95ECD173F855}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{22A35704-1763-48AE-B42C-6055B85060D0}" name="STT" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{7A6BB185-40B8-42E1-849C-59E116A4C578}" name="Công việc" dataDxfId="8"/>
@@ -776,26 +803,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7C54CA-71C9-4527-A841-C8DE308978A6}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.28515625" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
@@ -808,8 +836,9 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -822,11 +851,12 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
-    </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
@@ -839,8 +869,9 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
-    </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="K4" s="10"/>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -872,7 +903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" ht="33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -897,10 +928,12 @@
       <c r="H7" s="9">
         <v>44074</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="9">
+        <v>44118</v>
+      </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -930,7 +963,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6" t="s">
@@ -951,10 +984,12 @@
       <c r="H9" s="9">
         <v>44095</v>
       </c>
-      <c r="I9" s="9"/>
+      <c r="I9" s="9">
+        <v>44105</v>
+      </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -982,7 +1017,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1012,399 +1047,599 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="9">
-        <v>44101</v>
-      </c>
-      <c r="G12" s="9">
-        <v>44103</v>
-      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="9">
-        <v>44108</v>
-      </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="9">
-        <v>44103</v>
-      </c>
-      <c r="G13" s="9">
-        <v>44105</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>44124</v>
+      </c>
+      <c r="I12" s="9">
+        <v>44126</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5">
+        <v>6</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
+        <v>44124</v>
+      </c>
+      <c r="I13" s="9">
+        <v>44126</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="9">
-        <v>44105</v>
-      </c>
-      <c r="G14" s="9">
-        <v>44109</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="9">
-        <v>44109</v>
-      </c>
-      <c r="G15" s="9">
-        <v>44112</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="9">
-        <v>44112</v>
-      </c>
-      <c r="G16" s="9">
-        <v>44114</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="9">
-        <v>44114</v>
-      </c>
-      <c r="G17" s="9">
-        <v>44117</v>
-      </c>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="9">
-        <v>44117</v>
-      </c>
-      <c r="G18" s="9">
-        <v>44122</v>
-      </c>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="9">
-        <v>44122</v>
-      </c>
-      <c r="G19" s="9">
+        <v>48</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
         <v>44127</v>
       </c>
+      <c r="I14" s="9">
+        <v>44137</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="5">
+        <v>8</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9">
+        <v>44127</v>
+      </c>
+      <c r="I15" s="9">
+        <v>44137</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>9</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9">
+        <v>44127</v>
+      </c>
+      <c r="I16" s="9">
+        <v>44137</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9">
+        <v>44127</v>
+      </c>
+      <c r="I17" s="9">
+        <v>44137</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>11</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9">
+        <v>44127</v>
+      </c>
+      <c r="I18" s="9">
+        <v>44137</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>12</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="9">
+        <v>44147</v>
+      </c>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="9">
-        <v>44127</v>
-      </c>
-      <c r="G20" s="9">
-        <v>44130</v>
-      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
+    <row r="21" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="F21" s="9">
-        <v>44130</v>
+        <v>44101</v>
       </c>
       <c r="G21" s="9">
-        <v>44136</v>
-      </c>
-      <c r="H21" s="9"/>
+        <v>44103</v>
+      </c>
+      <c r="H21" s="9">
+        <v>44108</v>
+      </c>
       <c r="I21" s="9"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="5"/>
       <c r="F22" s="9">
-        <v>44136</v>
+        <v>44103</v>
       </c>
       <c r="G22" s="9">
-        <v>44140</v>
+        <v>44105</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6" t="s">
-        <v>34</v>
+    <row r="23" spans="1:10" s="1" customFormat="1" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F23" s="9">
-        <v>44140</v>
+        <v>44105</v>
       </c>
       <c r="G23" s="9">
-        <v>44145</v>
+        <v>44109</v>
       </c>
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="F24" s="9">
-        <v>44145</v>
+        <v>44109</v>
       </c>
       <c r="G24" s="9">
-        <v>44150</v>
+        <v>44112</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F25" s="9">
-        <v>44150</v>
+        <v>44112</v>
       </c>
       <c r="G25" s="9">
-        <v>44155</v>
+        <v>44114</v>
       </c>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="E26" s="5"/>
       <c r="F26" s="9">
-        <v>44155</v>
+        <v>44114</v>
       </c>
       <c r="G26" s="9">
-        <v>44160</v>
+        <v>44117</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>7</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="6"/>
+    <row r="27" spans="1:10" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D27" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="9">
-        <v>44160</v>
+        <v>44117</v>
       </c>
       <c r="G27" s="9">
-        <v>44162</v>
+        <v>44122</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>8</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>39</v>
-      </c>
+    <row r="28" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>43</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D28" s="5"/>
       <c r="E28" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F28" s="9">
-        <v>44162</v>
+        <v>44122</v>
       </c>
       <c r="G28" s="9">
-        <v>44167</v>
+        <v>44127</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" s="1" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>9</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C29" s="6"/>
+    <row r="29" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="D29" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>43</v>
-      </c>
+      <c r="E29" s="5"/>
       <c r="F29" s="9">
-        <v>44162</v>
+        <v>44127</v>
       </c>
       <c r="G29" s="9">
-        <v>44171</v>
+        <v>44130</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="5"/>
     </row>
+    <row r="30" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="9">
+        <v>44130</v>
+      </c>
+      <c r="G30" s="9">
+        <v>44136</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="9">
+        <v>44136</v>
+      </c>
+      <c r="G31" s="9">
+        <v>44140</v>
+      </c>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="9">
+        <v>44140</v>
+      </c>
+      <c r="G32" s="9">
+        <v>44145</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="9">
+        <v>44145</v>
+      </c>
+      <c r="G33" s="9">
+        <v>44150</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="9">
+        <v>44150</v>
+      </c>
+      <c r="G34" s="9">
+        <v>44155</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="9">
+        <v>44155</v>
+      </c>
+      <c r="G35" s="9">
+        <v>44160</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>7</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="6"/>
+      <c r="D36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F36" s="9">
+        <v>44160</v>
+      </c>
+      <c r="G36" s="9">
+        <v>44162</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>8</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="9">
+        <v>44162</v>
+      </c>
+      <c r="G37" s="9">
+        <v>44167</v>
+      </c>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" s="1" customFormat="1" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>9</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="9">
+        <v>44162</v>
+      </c>
+      <c r="G38" s="9">
+        <v>44171</v>
+      </c>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A4:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>